<commit_message>
Mittlerer Fehler über alle 46 Punkte
</commit_message>
<xml_diff>
--- a/data/output/k Werte Vergleich.xlsx
+++ b/data/output/k Werte Vergleich.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scheide\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scheide\Desktop\Degi Stuff\Un\Abgeschlossen\eclipse\new-workspace\WiFi Location Fingerprinting\data\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81E9BFDE-A9A2-42A6-9E3D-329A80C28DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858EF3E6-297B-47F5-AF36-8E3D18877683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="61">
   <si>
     <t>k=1</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>P35</t>
+  </si>
+  <si>
+    <t>Gesamt</t>
   </si>
 </sst>
 </file>
@@ -4182,6 +4185,530 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Mittlerehr</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> Fehler aller 46 Punkte</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Vergleich!$W$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Vergleich!$X$65:$AE$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.3913043478260869</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4413043478260867</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.661956521739131</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3902173913043478</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2934782608695636</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3043478260869561</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4467391304347821</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-92E7-485B-B3AD-2E963E1368FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Vergleich!$W$115</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Empirical</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Vergleich!$X$115:$AE$115</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.1173913043478261</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6532608695652176</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.480434782608695</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5456521739130435</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.743478260869566</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8760869565217386</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.68695652173913</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7086956521739132</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-92E7-485B-B3AD-2E963E1368FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="854361071"/>
+        <c:axId val="854364399"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="854361071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>k</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="854364399"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="854364399"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Distanz</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> in m</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="854361071"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -17799,6 +18326,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -19139,6 +19706,509 @@
 </file>
 
 <file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -24113,6 +25183,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>271462</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Diagramm 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4407AD4-4504-4945-95F3-E9FC2D056333}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -24415,8 +25521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I48" sqref="A1:I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25840,8 +26946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2495D8DC-D1E4-49CB-A811-1FEFE85EAC03}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I48" sqref="A1:I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27253,10 +28359,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B4CBB1E-480E-4B88-ABA4-096EEE624308}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:AE115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27367,7 +28473,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>55</v>
       </c>
@@ -27396,7 +28502,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
@@ -27424,13 +28530,384 @@
       <c r="I18" s="1">
         <v>2.4</v>
       </c>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE18" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X19" s="1">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>9.35</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>9.25</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>9.35</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>9.35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="X20" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="X21" s="1">
+        <v>7.35</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>7.55</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>7.15</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>7.35</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="AD21" s="1">
+        <v>7.45</v>
+      </c>
+      <c r="AE21" s="1">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="X22" s="1">
+        <v>6.45</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>6.85</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>6.45</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>6.85</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>6.35</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="X23" s="1">
+        <v>8.65</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="Z23" s="1">
+        <v>8.65</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>8.65</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>8.75</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>8.65</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X24" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>6.25</v>
+      </c>
+      <c r="Z24" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>7.25</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="X25" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>6.45</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>7.05</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>6.35</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="X26" s="1">
+        <v>5.85</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>7</v>
+      </c>
+      <c r="Z26" s="1">
+        <v>5.65</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="AD26" s="1">
+        <v>5.85</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X27" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="Y27" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="AC27" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="AD27" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="X28" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="Y28" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="Z28" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AC28" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="AD28" s="1">
+        <v>3.35</v>
+      </c>
+      <c r="AE28" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="X29" s="1">
+        <v>6.25</v>
+      </c>
+      <c r="Y29" s="1">
+        <v>6.35</v>
+      </c>
+      <c r="Z29" s="1">
+        <v>6.35</v>
+      </c>
+      <c r="AA29" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="AB29" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="AC29" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="AD29" s="1">
+        <v>7.05</v>
+      </c>
+      <c r="AE29" s="1">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>58</v>
       </c>
+      <c r="W30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X30" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="Y30" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="Z30" s="1">
+        <v>7.15</v>
+      </c>
+      <c r="AA30" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="AC30" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="AD30" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="AE30" s="1">
+        <v>6.9</v>
+      </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>55</v>
       </c>
@@ -27458,8 +28935,35 @@
       <c r="I31" s="1">
         <v>6.9</v>
       </c>
+      <c r="W31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="X31" s="1">
+        <v>7.55</v>
+      </c>
+      <c r="Y31" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="Z31" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="AC31" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="AD31" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="AE31" s="1">
+        <v>7.1</v>
+      </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>56</v>
       </c>
@@ -27487,13 +28991,444 @@
       <c r="I32" s="1">
         <v>1.25</v>
       </c>
+      <c r="W32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X32" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y32" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="Z32" s="1">
+        <v>8.65</v>
+      </c>
+      <c r="AA32" s="1">
+        <v>7.35</v>
+      </c>
+      <c r="AB32" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="AC32" s="1">
+        <v>6.25</v>
+      </c>
+      <c r="AD32" s="1">
+        <v>7.25</v>
+      </c>
+      <c r="AE32" s="1">
+        <v>6.65</v>
+      </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X33" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="Y33" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="Z33" s="1">
+        <v>6.25</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>7.05</v>
+      </c>
+      <c r="AB33" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="AC33" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="AD33" s="1">
+        <v>5.95</v>
+      </c>
+      <c r="AE33" s="1">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="X34" s="1">
+        <v>2.95</v>
+      </c>
+      <c r="Y34" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="Z34" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AA34" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="AB34" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="AC34" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="AD34" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE34" s="1">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X35" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="Y35" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="Z35" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA35" s="1">
+        <v>5.85</v>
+      </c>
+      <c r="AB35" s="1">
+        <v>5.85</v>
+      </c>
+      <c r="AC35" s="1">
+        <v>5.65</v>
+      </c>
+      <c r="AD35" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="AE35" s="1">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X36" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="Y36" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="Z36" s="1">
+        <v>6.55</v>
+      </c>
+      <c r="AA36" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="AB36" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="AC36" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="AD36" s="1">
+        <v>8.65</v>
+      </c>
+      <c r="AE36" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W37" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X37" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="Y37" s="1">
+        <v>8.15</v>
+      </c>
+      <c r="Z37" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AA37" s="1">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="AB37" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="AC37" s="1">
+        <v>8.15</v>
+      </c>
+      <c r="AD37" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="AE37" s="1">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W38" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="X38" s="1">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="Y38" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="Z38" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="AA38" s="1">
+        <v>8.75</v>
+      </c>
+      <c r="AB38" s="1">
+        <v>8.75</v>
+      </c>
+      <c r="AC38" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="AD38" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="AE38" s="1">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X39" s="1">
+        <v>3.85</v>
+      </c>
+      <c r="Y39" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z39" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="AA39" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="AB39" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="AC39" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AD39" s="1">
+        <v>3.35</v>
+      </c>
+      <c r="AE39" s="1">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X40" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="Y40" s="1">
+        <v>2.15</v>
+      </c>
+      <c r="Z40" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="AA40" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="AB40" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC40" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AD40" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="AE40" s="1">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="X41" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="Y41" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="Z41" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="AA41" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="AB41" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="AC41" s="1">
+        <v>2.95</v>
+      </c>
+      <c r="AD41" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="AE41" s="1">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W42" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="X42" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="Y42" s="1">
+        <v>2.95</v>
+      </c>
+      <c r="Z42" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AA42" s="1">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AB42" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="AC42" s="1">
+        <v>1.65</v>
+      </c>
+      <c r="AD42" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="AE42" s="1">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X43" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="Y43" s="1">
+        <v>4.55</v>
+      </c>
+      <c r="Z43" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="AA43" s="1">
+        <v>3.45</v>
+      </c>
+      <c r="AB43" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="AC43" s="1">
+        <v>3.85</v>
+      </c>
+      <c r="AD43" s="1">
+        <v>4.45</v>
+      </c>
+      <c r="AE43" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W44" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X44" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="Y44" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="Z44" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AA44" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB44" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="AC44" s="1">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AD44" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="AE44" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="X45" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="Y45" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="Z45" s="1">
+        <v>3.55</v>
+      </c>
+      <c r="AA45" s="1">
+        <v>3.45</v>
+      </c>
+      <c r="AB45" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC45" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="AD45" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AE45" s="1">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>59</v>
       </c>
+      <c r="W46" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="X46" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="Y46" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z46" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="AA46" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AB46" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="AC46" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="AD46" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AE46" s="1">
+        <v>2.85</v>
+      </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>55</v>
       </c>
@@ -27521,8 +29456,35 @@
       <c r="I47" s="1">
         <v>4.2</v>
       </c>
+      <c r="W47" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X47" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y47" s="1">
+        <v>3.95</v>
+      </c>
+      <c r="Z47" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA47" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AB47" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="AC47" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="AD47" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="AE47" s="1">
+        <v>2.85</v>
+      </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
@@ -27549,6 +29511,1973 @@
       </c>
       <c r="I48" s="1">
         <v>3.5</v>
+      </c>
+      <c r="W48" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="X48" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y48" s="1">
+        <v>2.95</v>
+      </c>
+      <c r="Z48" s="1">
+        <v>4.05</v>
+      </c>
+      <c r="AA48" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AB48" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="AC48" s="1">
+        <v>3.85</v>
+      </c>
+      <c r="AD48" s="1">
+        <v>2.85</v>
+      </c>
+      <c r="AE48" s="1">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W49" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="X49" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Y49" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="Z49" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA49" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="AB49" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="AC49" s="1">
+        <v>2.15</v>
+      </c>
+      <c r="AD49" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="AE49" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W50" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X50" s="1">
+        <v>4.55</v>
+      </c>
+      <c r="Y50" s="1">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="Z50" s="1">
+        <v>2.85</v>
+      </c>
+      <c r="AA50" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="AB50" s="1">
+        <v>3.05</v>
+      </c>
+      <c r="AC50" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="AD50" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="AE50" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W51" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X51" s="1">
+        <v>2.95</v>
+      </c>
+      <c r="Y51" s="1">
+        <v>3.45</v>
+      </c>
+      <c r="Z51" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="AA51" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="AB51" s="1">
+        <v>4.45</v>
+      </c>
+      <c r="AC51" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="AD51" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="AE51" s="1">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W52" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X52" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y52" s="1">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="Z52" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="AA52" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="AB52" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="AC52" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AD52" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="AE52" s="1">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W53" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X53" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y53" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="Z53" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="AA53" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="AB53" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC53" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="AD53" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AE53" s="1">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W54" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X54" s="1">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="Y54" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="Z54" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="AA54" s="1">
+        <v>3.55</v>
+      </c>
+      <c r="AB54" s="1">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="AC54" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="AD54" s="1">
+        <v>5.15</v>
+      </c>
+      <c r="AE54" s="1">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W55" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X55" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="Y55" s="1">
+        <v>4.55</v>
+      </c>
+      <c r="Z55" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="AA55" s="1">
+        <v>5.05</v>
+      </c>
+      <c r="AB55" s="1">
+        <v>4.75</v>
+      </c>
+      <c r="AC55" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="AD55" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="AE55" s="1">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W56" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X56" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="Y56" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="Z56" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="AA56" s="1">
+        <v>5.75</v>
+      </c>
+      <c r="AB56" s="1">
+        <v>5.45</v>
+      </c>
+      <c r="AC56" s="1">
+        <v>5.45</v>
+      </c>
+      <c r="AD56" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="AE56" s="1">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W57" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X57" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="Y57" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Z57" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="AA57" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="AB57" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="AC57" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="AD57" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="AE57" s="1">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W58" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="X58" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="Y58" s="1">
+        <v>8.35</v>
+      </c>
+      <c r="Z58" s="1">
+        <v>8.65</v>
+      </c>
+      <c r="AA58" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="AB58" s="1">
+        <v>7.45</v>
+      </c>
+      <c r="AC58" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="AD58" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="AE58" s="1">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W59" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="X59" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="Y59" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="Z59" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="AA59" s="1">
+        <v>9</v>
+      </c>
+      <c r="AB59" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC59" s="1">
+        <v>10.15</v>
+      </c>
+      <c r="AD59" s="1">
+        <v>9.35</v>
+      </c>
+      <c r="AE59" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W60" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="X60" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Y60" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="Z60" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="AA60" s="1">
+        <v>3.85</v>
+      </c>
+      <c r="AB60" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="AC60" s="1">
+        <v>5.35</v>
+      </c>
+      <c r="AD60" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="AE60" s="1">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W61" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="X61" s="1">
+        <v>6.35</v>
+      </c>
+      <c r="Y61" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="Z61" s="1">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="AA61" s="1">
+        <v>5.75</v>
+      </c>
+      <c r="AB61" s="1">
+        <v>5.95</v>
+      </c>
+      <c r="AC61" s="1">
+        <v>5.75</v>
+      </c>
+      <c r="AD61" s="1">
+        <v>6.35</v>
+      </c>
+      <c r="AE61" s="1">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W62" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X62" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="Y62" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="Z62" s="1">
+        <v>3.55</v>
+      </c>
+      <c r="AA62" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AB62" s="1">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="AC62" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AD62" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="AE62" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="W63" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X63" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="Y63" s="1">
+        <v>5.35</v>
+      </c>
+      <c r="Z63" s="1">
+        <v>5.85</v>
+      </c>
+      <c r="AA63" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="AB63" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="AC63" s="1">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="AD63" s="1">
+        <v>5.15</v>
+      </c>
+      <c r="AE63" s="1">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>55</v>
+      </c>
+      <c r="B64">
+        <f>AVERAGE(B18:B63)</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C64">
+        <f t="shared" ref="C64:I64" si="0">AVERAGE(C18:C63)</f>
+        <v>4.2</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="0"/>
+        <v>3.63</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>3.5699999999999994</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="0"/>
+        <v>3.45</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="0"/>
+        <v>3.3299999999999996</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="0"/>
+        <v>3.65</v>
+      </c>
+      <c r="W64" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X64" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="Y64" s="1">
+        <v>7.65</v>
+      </c>
+      <c r="Z64" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="AA64" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="AB64" s="1">
+        <v>6.85</v>
+      </c>
+      <c r="AC64" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="AD64" s="1">
+        <v>7.25</v>
+      </c>
+      <c r="AE64" s="1">
+        <v>7.55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>56</v>
+      </c>
+      <c r="W65" t="s">
+        <v>55</v>
+      </c>
+      <c r="X65">
+        <f>AVERAGE(X19:X64)</f>
+        <v>5.3913043478260869</v>
+      </c>
+      <c r="Y65">
+        <f t="shared" ref="Y65:AE65" si="1">AVERAGE(Y19:Y64)</f>
+        <v>5.4413043478260867</v>
+      </c>
+      <c r="Z65">
+        <f t="shared" si="1"/>
+        <v>5.661956521739131</v>
+      </c>
+      <c r="AA65">
+        <f t="shared" si="1"/>
+        <v>5.3902173913043478</v>
+      </c>
+      <c r="AB65">
+        <f t="shared" si="1"/>
+        <v>5.2934782608695636</v>
+      </c>
+      <c r="AC65">
+        <f t="shared" si="1"/>
+        <v>5.3043478260869561</v>
+      </c>
+      <c r="AD65">
+        <f t="shared" si="1"/>
+        <v>5.4467391304347821</v>
+      </c>
+      <c r="AE65">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W68" s="1"/>
+      <c r="X68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y68" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z68" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC68" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE68" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X69" s="1">
+        <v>5.75</v>
+      </c>
+      <c r="Y69" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Z69" s="1">
+        <v>4.95</v>
+      </c>
+      <c r="AA69" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="AB69" s="1">
+        <v>4.95</v>
+      </c>
+      <c r="AC69" s="1">
+        <v>5.45</v>
+      </c>
+      <c r="AD69" s="1">
+        <v>5</v>
+      </c>
+      <c r="AE69" s="1">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="X70" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y70" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="Z70" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="AA70" s="1">
+        <v>2.35</v>
+      </c>
+      <c r="AB70" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="AC70" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AD70" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="AE70" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W71" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X71" s="1">
+        <v>3.35</v>
+      </c>
+      <c r="Y71" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="Z71" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="AA71" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AB71" s="1">
+        <v>4.05</v>
+      </c>
+      <c r="AC71" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AD71" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="AE71" s="1">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X72" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Y72" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="Z72" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA72" s="1">
+        <v>2.35</v>
+      </c>
+      <c r="AB72" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="AC72" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="AD72" s="1">
+        <v>2.85</v>
+      </c>
+      <c r="AE72" s="1">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X73" s="1">
+        <v>4.75</v>
+      </c>
+      <c r="Y73" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="Z73" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="AA73" s="1">
+        <v>1.35</v>
+      </c>
+      <c r="AB73" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="AC73" s="1">
+        <v>2.95</v>
+      </c>
+      <c r="AD73" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AE73" s="1">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W74" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X74" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="Y74" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="Z74" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AA74" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AB74" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="AC74" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="AD74" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="AE74" s="1">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W75" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X75" s="1">
+        <v>2.35</v>
+      </c>
+      <c r="Y75" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Z75" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AA75" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="AB75" s="1">
+        <v>1.35</v>
+      </c>
+      <c r="AC75" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD75" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="AE75" s="1">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W76" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X76" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="Y76" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="Z76" s="1">
+        <v>1.55</v>
+      </c>
+      <c r="AA76" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="AB76" s="1">
+        <v>2.35</v>
+      </c>
+      <c r="AC76" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="AD76" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AE76" s="1">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X77" s="1">
+        <v>3.95</v>
+      </c>
+      <c r="Y77" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="Z77" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="AA77" s="1">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="AB77" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="AC77" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD77" s="1">
+        <v>4.05</v>
+      </c>
+      <c r="AE77" s="1">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="X78" s="1">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="Y78" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="Z78" s="1">
+        <v>2.35</v>
+      </c>
+      <c r="AA78" s="1">
+        <v>3.55</v>
+      </c>
+      <c r="AB78" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="AC78" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="AD78" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="AE78" s="1">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W79" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X79" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="Y79" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="Z79" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="AA79" s="1">
+        <v>3.35</v>
+      </c>
+      <c r="AB79" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AC79" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="AD79" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AE79" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W80" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X80" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y80" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="Z80" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="AA80" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="AB80" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC80" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AD80" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AE80" s="1">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="81" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W81" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X81" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="Y81" s="1">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="Z81" s="1">
+        <v>3.85</v>
+      </c>
+      <c r="AA81" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="AB81" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="AC81" s="1">
+        <v>7.55</v>
+      </c>
+      <c r="AD81" s="1">
+        <v>6.35</v>
+      </c>
+      <c r="AE81" s="1">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="82" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W82" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X82" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="Y82" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="Z82" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="AA82" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="AB82" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="AC82" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="AD82" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="AE82" s="1">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="83" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W83" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X83" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="Y83" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="Z83" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="AA83" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AB83" s="1">
+        <v>4.55</v>
+      </c>
+      <c r="AC83" s="1">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="AD83" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="AE83" s="1">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W84" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X84" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="Y84" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="Z84" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="AA84" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="AB84" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AC84" s="1">
+        <v>2.15</v>
+      </c>
+      <c r="AD84" s="1">
+        <v>3.05</v>
+      </c>
+      <c r="AE84" s="1">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="85" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W85" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X85" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Y85" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="Z85" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA85" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AB85" s="1">
+        <v>1.85</v>
+      </c>
+      <c r="AC85" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AD85" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AE85" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W86" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X86" s="1">
+        <v>3.95</v>
+      </c>
+      <c r="Y86" s="1">
+        <v>2.35</v>
+      </c>
+      <c r="Z86" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="AA86" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="AB86" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AC86" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="AD86" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AE86" s="1">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="87" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W87" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X87" s="1">
+        <v>2.35</v>
+      </c>
+      <c r="Y87" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Z87" s="1">
+        <v>1.35</v>
+      </c>
+      <c r="AA87" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AB87" s="1">
+        <v>2.15</v>
+      </c>
+      <c r="AC87" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="AD87" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="AE87" s="1">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="88" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W88" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X88" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="Y88" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="Z88" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="AA88" s="1">
+        <v>3.35</v>
+      </c>
+      <c r="AB88" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="AC88" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="AD88" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE88" s="1">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="89" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W89" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X89" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="Y89" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="Z89" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="AA89" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="AB89" s="1">
+        <v>1.85</v>
+      </c>
+      <c r="AC89" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AD89" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AE89" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W90" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X90" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="Y90" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z90" s="1">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AA90" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="AB90" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="AC90" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AD90" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="AE90" s="1">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="91" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W91" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X91" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="Y91" s="1">
+        <v>1.85</v>
+      </c>
+      <c r="Z91" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="AA91" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="AB91" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AC91" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AD91" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="AE91" s="1">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="92" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W92" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X92" s="1">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="Y92" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="Z92" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="AA92" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="AB92" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="AC92" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="AD92" s="1">
+        <v>1.35</v>
+      </c>
+      <c r="AE92" s="1">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="93" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W93" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X93" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="Y93" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="Z93" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AA93" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="AB93" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="AC93" s="1">
+        <v>3.15</v>
+      </c>
+      <c r="AD93" s="1">
+        <v>4.55</v>
+      </c>
+      <c r="AE93" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W94" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X94" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="Y94" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="Z94" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="AA94" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="AB94" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC94" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="AD94" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="AE94" s="1">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="95" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W95" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X95" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="Y95" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="Z95" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AA95" s="1">
+        <v>1.65</v>
+      </c>
+      <c r="AB95" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AC95" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AD95" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AE95" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W96" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X96" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="Y96" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="Z96" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="AA96" s="1">
+        <v>2.95</v>
+      </c>
+      <c r="AB96" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC96" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AD96" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="AE96" s="1">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="97" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W97" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X97" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Y97" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="Z97" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AA97" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AB97" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AC97" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AD97" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="AE97" s="1">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="98" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W98" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X98" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="Y98" s="1">
+        <v>3.15</v>
+      </c>
+      <c r="Z98" s="1">
+        <v>2.85</v>
+      </c>
+      <c r="AA98" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="AB98" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="AC98" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AD98" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AE98" s="1">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="99" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W99" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X99" s="1">
+        <v>2.85</v>
+      </c>
+      <c r="Y99" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="Z99" s="1">
+        <v>1.85</v>
+      </c>
+      <c r="AA99" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="AB99" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="AC99" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="AD99" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AE99" s="1">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="100" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W100" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X100" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="Y100" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Z100" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="AA100" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="AB100" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AC100" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AD100" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AE100" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="101" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X101" s="1">
+        <v>2.15</v>
+      </c>
+      <c r="Y101" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="Z101" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="AA101" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="AB101" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AC101" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="AD101" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="AE101" s="1">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="102" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W102" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X102" s="1">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="Y102" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="Z102" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AA102" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AB102" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AC102" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AD102" s="1">
+        <v>2.15</v>
+      </c>
+      <c r="AE102" s="1">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="103" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W103" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X103" s="1">
+        <v>5.75</v>
+      </c>
+      <c r="Y103" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Z103" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="AA103" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AB103" s="1">
+        <v>3.55</v>
+      </c>
+      <c r="AC103" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="AD103" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="AE103" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="104" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W104" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X104" s="1">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="Y104" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="Z104" s="1">
+        <v>3.05</v>
+      </c>
+      <c r="AA104" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="AB104" s="1">
+        <v>4.05</v>
+      </c>
+      <c r="AC104" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="AD104" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="AE104" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="105" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W105" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X105" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="Y105" s="1">
+        <v>3.15</v>
+      </c>
+      <c r="Z105" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AA105" s="1">
+        <v>3.35</v>
+      </c>
+      <c r="AB105" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AC105" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="AD105" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AE105" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="106" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W106" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X106" s="1">
+        <v>3.05</v>
+      </c>
+      <c r="Y106" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="Z106" s="1">
+        <v>2.35</v>
+      </c>
+      <c r="AA106" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AB106" s="1">
+        <v>2.15</v>
+      </c>
+      <c r="AC106" s="1">
+        <v>1.65</v>
+      </c>
+      <c r="AD106" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="AE106" s="1">
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="107" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W107" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X107" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="Y107" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="Z107" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AA107" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AB107" s="1">
+        <v>2.15</v>
+      </c>
+      <c r="AC107" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="AD107" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="AE107" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="108" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W108" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X108" s="1">
+        <v>3.15</v>
+      </c>
+      <c r="Y108" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="Z108" s="1">
+        <v>2.15</v>
+      </c>
+      <c r="AA108" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AB108" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="AC108" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AD108" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="AE108" s="1">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="109" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W109" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="X109" s="1">
+        <v>3.05</v>
+      </c>
+      <c r="Y109" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="Z109" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA109" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AB109" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AC109" s="1">
+        <v>3.95</v>
+      </c>
+      <c r="AD109" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE109" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="110" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W110" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X110" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="Y110" s="1">
+        <v>2.85</v>
+      </c>
+      <c r="Z110" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA110" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AB110" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="AC110" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AD110" s="1">
+        <v>2.85</v>
+      </c>
+      <c r="AE110" s="1">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="111" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W111" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="X111" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="Y111" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="Z111" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AA111" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AB111" s="1">
+        <v>2.15</v>
+      </c>
+      <c r="AC111" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="AD111" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="AE111" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W112" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X112" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Y112" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z112" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="AA112" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="AB112" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="AC112" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="AD112" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="AE112" s="1">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="113" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W113" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X113" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="Y113" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Z113" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="AA113" s="1">
+        <v>1.85</v>
+      </c>
+      <c r="AB113" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC113" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="AD113" s="1">
+        <v>3.35</v>
+      </c>
+      <c r="AE113" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="114" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W114" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X114" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="Y114" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="Z114" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="AA114" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="AB114" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="AC114" s="1">
+        <v>2.95</v>
+      </c>
+      <c r="AD114" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="AE114" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="115" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W115" t="s">
+        <v>56</v>
+      </c>
+      <c r="X115">
+        <f>AVERAGE(X69:X114)</f>
+        <v>3.1173913043478261</v>
+      </c>
+      <c r="Y115">
+        <f t="shared" ref="Y115:AE115" si="2">AVERAGE(Y69:Y114)</f>
+        <v>2.6532608695652176</v>
+      </c>
+      <c r="Z115">
+        <f t="shared" si="2"/>
+        <v>2.480434782608695</v>
+      </c>
+      <c r="AA115">
+        <f t="shared" si="2"/>
+        <v>2.5456521739130435</v>
+      </c>
+      <c r="AB115">
+        <f t="shared" si="2"/>
+        <v>2.743478260869566</v>
+      </c>
+      <c r="AC115">
+        <f t="shared" si="2"/>
+        <v>2.8760869565217386</v>
+      </c>
+      <c r="AD115">
+        <f t="shared" si="2"/>
+        <v>2.68695652173913</v>
+      </c>
+      <c r="AE115">
+        <f t="shared" si="2"/>
+        <v>2.7086956521739132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>